<commit_message>
this is a checkpoint, revert back to here if needed
</commit_message>
<xml_diff>
--- a/test_results/pipeline_output/statements_shp-afs-2025.xlsx
+++ b/test_results/pipeline_output/statements_shp-afs-2025.xlsx
@@ -527,7 +527,7 @@
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>2026-02-23 16:17:31</t>
+          <t>2026-02-24 11:33:17</t>
         </is>
       </c>
     </row>
@@ -539,7 +539,7 @@
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>8728c11f-88e8-4fda-b67c-4700fd248a6a</t>
+          <t>160e6b94-fc98-450c-bf86-de6dd890286a</t>
         </is>
       </c>
     </row>

</xml_diff>